<commit_message>
Updating metadata for example data set UCP1KO
</commit_message>
<xml_diff>
--- a/example_data/UCP1KO/example_metadata_1.xlsx
+++ b/example_data/UCP1KO/example_metadata_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="173">
   <si>
     <t xml:space="preserve">Original_Column</t>
   </si>
@@ -109,25 +109,25 @@
     <t xml:space="preserve">Title</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter name of experiment</t>
+    <t xml:space="preserve">UCP1KO</t>
   </si>
   <si>
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-10-23</t>
+    <t xml:space="preserve">2024-11-11</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter your name</t>
+    <t xml:space="preserve">Martin Klingenspor</t>
   </si>
   <si>
     <t xml:space="preserve">Group</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter your working group</t>
+    <t xml:space="preserve">Klingenspor, TUM</t>
   </si>
   <si>
     <t xml:space="preserve">Sample-Section</t>
@@ -388,40 +388,52 @@
     <t xml:space="preserve">lm_end</t>
   </si>
   <si>
-    <t xml:space="preserve">18.2825451</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17.968895</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.223175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.9940205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.014164</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.0537338</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.5371399</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.5609322</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.2504196</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16.916605</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.7803593</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.0227833</t>
+    <t xml:space="preserve">16.26321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.69135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.39800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.51941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.28255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.96889</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.22318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.99402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.01416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.05373</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.53714</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.56093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.25042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.91661</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.78036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.02278</t>
   </si>
   <si>
     <t xml:space="preserve">fm_start</t>
@@ -478,13 +490,25 @@
     <t xml:space="preserve">fm_end</t>
   </si>
   <si>
-    <t xml:space="preserve">13.6194038</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.1043549</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.2898989</t>
+    <t xml:space="preserve"> 5.864944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.234464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.797132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.065608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.619404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.104355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.289899</t>
   </si>
   <si>
     <t xml:space="preserve">11.445715</t>
@@ -493,25 +517,25 @@
     <t xml:space="preserve">14.841568</t>
   </si>
   <si>
-    <t xml:space="preserve">13.7720451</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.2328596</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.0704145</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.4404888</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.6025133</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.1484003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14.8256168</t>
+    <t xml:space="preserve">13.772045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.232860</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.070415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.440489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.602513</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.148400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.825617</t>
   </si>
   <si>
     <t xml:space="preserve">Sub-Sample Section</t>
@@ -627,7 +651,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23:E23"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1136,7 +1160,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>104</v>
       </c>
@@ -1189,168 +1213,168 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>121</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="O21" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="P21" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="Q21" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="O22" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="P22" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="Q22" s="0" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="O23" s="0" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="P23" s="0" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="Q23" s="0" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>